<commit_message>
first commit o the week
</commit_message>
<xml_diff>
--- a/data/MG_LCLUC_Survey_Codebook_06.18.2025.xlsx
+++ b/data/MG_LCLUC_Survey_Codebook_06.18.2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jessi\OneDrive - Cornell University\Documents\MSPhD\AllingtonLab_LCLUC\RStudio_WorkingDirectory\MG_LCLUC_jessie\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8BFBAC24-2E78-41DC-8CB0-FCBBA015E753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE708AFF-1AB7-45AF-A7EE-5F1332BCC5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="2556" windowWidth="21516" windowHeight="9840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -4739,8 +4739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J328"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A267" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A279" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C291" sqref="C291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7067,7 +7067,7 @@
       <c r="A133" t="s">
         <v>35</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B133" s="15" t="s">
         <v>350</v>
       </c>
       <c r="C133" s="39" t="s">

</xml_diff>